<commit_message>
Updated XML comments. Removed redundant files.
</commit_message>
<xml_diff>
--- a/path parsing.xlsx
+++ b/path parsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="77">
   <si>
     <t>Search</t>
   </si>
@@ -231,7 +231,31 @@
     <t>GotGreaterThan</t>
   </si>
   <si>
-    <t>GotBang</t>
+    <t>ValueOrOperator</t>
+  </si>
+  <si>
+    <t>GotNot</t>
+  </si>
+  <si>
+    <t>Comparison</t>
+  </si>
+  <si>
+    <t>FinalizeComparison</t>
+  </si>
+  <si>
+    <t>GotCurrent</t>
+  </si>
+  <si>
+    <t>GotRoot</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>GotString</t>
+  </si>
+  <si>
+    <t>NumberOrPath</t>
   </si>
 </sst>
 </file>
@@ -295,7 +319,98 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -593,21 +708,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="topRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="3" customWidth="1"/>
-    <col min="2" max="13" width="19.85546875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="14" width="19.85546875" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -615,68 +730,74 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
@@ -684,104 +805,110 @@
         <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -789,47 +916,52 @@
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -840,31 +972,35 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="5"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="5"/>
+      <c r="N16" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -872,91 +1008,97 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="5"/>
+      <c r="L17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -967,45 +1109,47 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="5"/>
+      <c r="M22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1014,57 +1158,65 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="5"/>
+      <c r="K24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="5"/>
+      <c r="G25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:M12 B15:M25">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+  <conditionalFormatting sqref="B2:B12 B15:B25 D2:N12 D15:N25">
+    <cfRule type="containsBlanks" dxfId="10" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C12 C15:C25">
+    <cfRule type="containsBlanks" dxfId="9" priority="1">
+      <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1074,17 +1226,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6:N6"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="3" customWidth="1"/>
-    <col min="2" max="19" width="19.85546875" style="4" customWidth="1"/>
+    <col min="2" max="14" width="18.85546875" style="4" customWidth="1"/>
+    <col min="15" max="19" width="19.85546875" style="4" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -1131,7 +1284,9 @@
       <c r="N1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -1158,157 +1313,262 @@
       <c r="J3" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="O3" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="O11" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:S4">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B5:J6 O5:S6 B7:S7 B2:S4">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:S9">
+  <conditionalFormatting sqref="B10:S13">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(B10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14 E14:I14 K14:N14 P14:S14">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(C14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:N5 K6 M6:N6">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(K5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(D14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(B14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(J14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(L6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O14">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B7))=0</formula>
+      <formula>LEN(TRIM(O14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added ability to reference root path in expressions. Disallowed '@' in root path during parsing.
</commit_message>
<xml_diff>
--- a/path parsing.xlsx
+++ b/path parsing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdennis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Manatee.Json\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="77">
   <si>
     <t>Search</t>
   </si>
@@ -207,9 +207,6 @@
     <t>GotExponent</t>
   </si>
   <si>
-    <t>GotPath</t>
-  </si>
-  <si>
     <t>LessThan</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>NumberOrPath</t>
+  </si>
+  <si>
+    <t>Root</t>
   </si>
 </sst>
 </file>
@@ -319,7 +319,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -957,10 +992,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1210,12 +1245,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B12 B15:B25 D2:N12 D15:N25">
-    <cfRule type="containsBlanks" dxfId="10" priority="2">
+    <cfRule type="containsBlanks" dxfId="20" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C12 C15:C25">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
+    <cfRule type="containsBlanks" dxfId="19" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1226,22 +1261,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O14" sqref="O14"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="3" customWidth="1"/>
-    <col min="2" max="14" width="18.85546875" style="4" customWidth="1"/>
-    <col min="15" max="19" width="19.85546875" style="4" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="15" width="18.85546875" style="4" customWidth="1"/>
+    <col min="16" max="20" width="19.85546875" style="4" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1270,29 +1305,32 @@
         <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" s="1"/>
+      <c r="P1" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1300,7 +1338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>50</v>
       </c>
@@ -1313,13 +1351,16 @@
       <c r="J3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>51</v>
@@ -1330,8 +1371,11 @@
       <c r="J4" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1353,30 +1397,30 @@
       <c r="I5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>51</v>
@@ -1387,11 +1431,14 @@
       <c r="J7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="K7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1423,24 +1470,27 @@
         <v>48</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1448,7 +1498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1459,13 +1509,16 @@
         <v>54</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
@@ -1487,30 +1540,30 @@
       <c r="I12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="O12" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>52</v>
@@ -1519,56 +1572,74 @@
         <v>54</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="M14" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B5:J6 O5:S6 B7:S7 B2:S4">
-    <cfRule type="containsBlanks" dxfId="8" priority="9">
+  <conditionalFormatting sqref="P5:T6 B2:I7 K2:T4 K7:T7 K5:K6">
+    <cfRule type="containsBlanks" dxfId="18" priority="14">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:S13">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+  <conditionalFormatting sqref="B10:I13 K10:T13">
+    <cfRule type="containsBlanks" dxfId="17" priority="13">
       <formula>LEN(TRIM(B10))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14 E14:I14 K14:N14 P14:S14">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+  <conditionalFormatting sqref="C14 E14:I14 L14:O14 Q14:T14">
+    <cfRule type="containsBlanks" dxfId="16" priority="12">
       <formula>LEN(TRIM(C14))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:N5 K6 M6:N6">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(K5))=0</formula>
+  <conditionalFormatting sqref="L5:O5 L6 N6:O6">
+    <cfRule type="containsBlanks" dxfId="15" priority="11">
+      <formula>LEN(TRIM(L5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="14" priority="10">
       <formula>LEN(TRIM(D14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="13" priority="9">
       <formula>LEN(TRIM(B14))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M6">
+    <cfRule type="containsBlanks" dxfId="11" priority="7">
+      <formula>LEN(TRIM(M6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14">
+    <cfRule type="containsBlanks" dxfId="10" priority="6">
+      <formula>LEN(TRIM(P14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J7">
+    <cfRule type="containsBlanks" dxfId="9" priority="5">
+      <formula>LEN(TRIM(J2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J13">
+    <cfRule type="containsBlanks" dxfId="7" priority="4">
+      <formula>LEN(TRIM(J10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="2">
       <formula>LEN(TRIM(J14))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(L6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O14">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(O14))=0</formula>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(K14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed JsonPath.  Ready for release.
</commit_message>
<xml_diff>
--- a/path parsing.xlsx
+++ b/path parsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="83">
   <si>
     <t>Search</t>
   </si>
@@ -256,6 +256,24 @@
   </si>
   <si>
     <t>Root</t>
+  </si>
+  <si>
+    <t>BooleanOrComparison</t>
+  </si>
+  <si>
+    <t>GotNamedConstant</t>
+  </si>
+  <si>
+    <t>And</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>GotAnd</t>
+  </si>
+  <si>
+    <t>GotOr</t>
   </si>
 </sst>
 </file>
@@ -319,7 +337,238 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="54">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1245,12 +1494,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B12 B15:B25 D2:N12 D15:N25">
-    <cfRule type="containsBlanks" dxfId="20" priority="2">
+    <cfRule type="containsBlanks" dxfId="50" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C12 C15:C25">
-    <cfRule type="containsBlanks" dxfId="19" priority="1">
+    <cfRule type="containsBlanks" dxfId="49" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1261,17 +1510,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K14" sqref="K14"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="3" customWidth="1"/>
-    <col min="2" max="15" width="18.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="18.85546875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="20" width="19.85546875" style="4" customWidth="1"/>
     <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -1325,9 +1575,15 @@
       <c r="P1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1354,7 +1610,13 @@
       <c r="K3" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="O3" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="P3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1407,7 +1669,13 @@
         <v>67</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>67</v>
+        <v>77</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1417,6 +1685,12 @@
       <c r="M6" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="R6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1435,211 +1709,371 @@
         <v>51</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="P10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>66</v>
+        <v>50</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="P12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="Q16" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P5:T6 B2:I7 K2:T4 K7:T7 K5:K6">
-    <cfRule type="containsBlanks" dxfId="18" priority="14">
+  <conditionalFormatting sqref="P6:T6 K2:T2 L8 K5:K6 K7:L7 B2:I8 N7:T8 K4:T4 K3:N3 P3:T3 P5:Q5 T5">
+    <cfRule type="containsBlanks" dxfId="48" priority="32">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:I13 K10:T13">
-    <cfRule type="containsBlanks" dxfId="17" priority="13">
-      <formula>LEN(TRIM(B10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14 E14:I14 L14:O14 Q14:T14">
-    <cfRule type="containsBlanks" dxfId="16" priority="12">
-      <formula>LEN(TRIM(C14))=0</formula>
+  <conditionalFormatting sqref="B11:I12 B14:I15 K11:T12 K14:T15">
+    <cfRule type="containsBlanks" dxfId="47" priority="31">
+      <formula>LEN(TRIM(B11))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16 E16:I16 L16:O16 R16:T16">
+    <cfRule type="containsBlanks" dxfId="46" priority="30">
+      <formula>LEN(TRIM(C16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:O5 L6 N6:O6">
-    <cfRule type="containsBlanks" dxfId="15" priority="11">
+    <cfRule type="containsBlanks" dxfId="45" priority="29">
       <formula>LEN(TRIM(L5))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="containsBlanks" dxfId="14" priority="10">
-      <formula>LEN(TRIM(D14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="containsBlanks" dxfId="13" priority="9">
-      <formula>LEN(TRIM(B14))=0</formula>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="containsBlanks" dxfId="44" priority="28">
+      <formula>LEN(TRIM(D16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="containsBlanks" dxfId="43" priority="27">
+      <formula>LEN(TRIM(B16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="containsBlanks" dxfId="11" priority="7">
+    <cfRule type="containsBlanks" dxfId="42" priority="25">
       <formula>LEN(TRIM(M6))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P14">
-    <cfRule type="containsBlanks" dxfId="10" priority="6">
-      <formula>LEN(TRIM(P14))=0</formula>
+  <conditionalFormatting sqref="P16">
+    <cfRule type="containsBlanks" dxfId="41" priority="24">
+      <formula>LEN(TRIM(P16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J7">
-    <cfRule type="containsBlanks" dxfId="9" priority="5">
+    <cfRule type="containsBlanks" dxfId="40" priority="23">
       <formula>LEN(TRIM(J2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:J13">
-    <cfRule type="containsBlanks" dxfId="7" priority="4">
-      <formula>LEN(TRIM(J10))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
-    <cfRule type="containsBlanks" dxfId="3" priority="2">
-      <formula>LEN(TRIM(J14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(K14))=0</formula>
+  <conditionalFormatting sqref="J11:J12 J14:J15">
+    <cfRule type="containsBlanks" dxfId="39" priority="22">
+      <formula>LEN(TRIM(J11))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="containsBlanks" dxfId="38" priority="20">
+      <formula>LEN(TRIM(J16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="containsBlanks" dxfId="37" priority="19">
+      <formula>LEN(TRIM(K16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:I17 L17 R17:T17 N17:P17">
+    <cfRule type="containsBlanks" dxfId="36" priority="18">
+      <formula>LEN(TRIM(C17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7">
+    <cfRule type="containsBlanks" dxfId="34" priority="16">
+      <formula>LEN(TRIM(M7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:I13 K13:T13">
+    <cfRule type="containsBlanks" dxfId="33" priority="15">
+      <formula>LEN(TRIM(B13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="containsBlanks" dxfId="31" priority="14">
+      <formula>LEN(TRIM(J13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17">
+    <cfRule type="containsBlanks" dxfId="29" priority="13">
+      <formula>LEN(TRIM(Q17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="containsBlanks" dxfId="23" priority="10">
+      <formula>LEN(TRIM(J17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsBlanks" dxfId="21" priority="9">
+      <formula>LEN(TRIM(K17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsBlanks" dxfId="19" priority="8">
+      <formula>LEN(TRIM(B17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsBlanks" dxfId="16" priority="7">
+      <formula>LEN(TRIM(K8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="containsBlanks" dxfId="14" priority="6">
+      <formula>LEN(TRIM(J8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17">
+    <cfRule type="containsBlanks" dxfId="12" priority="5">
+      <formula>LEN(TRIM(M17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8">
+    <cfRule type="containsBlanks" dxfId="10" priority="4">
+      <formula>LEN(TRIM(M8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q16">
+    <cfRule type="containsBlanks" dxfId="7" priority="3">
+      <formula>LEN(TRIM(Q16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
+      <formula>LEN(TRIM(O3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:S5">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(R5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reorganized solution to allow easier loading/unloading of other frameworks. Updated JsonSerializationTypeRegistry to take the serializer as an argument.
</commit_message>
<xml_diff>
--- a/path parsing.xlsx
+++ b/path parsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="85">
   <si>
     <t>Search</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>GotOr</t>
+  </si>
+  <si>
+    <t>Operator/Function</t>
+  </si>
+  <si>
+    <t>GotFunction</t>
   </si>
 </sst>
 </file>
@@ -337,49 +343,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <fill>
         <patternFill>
@@ -996,7 +960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <selection pane="topRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,6 +1035,9 @@
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="J3" s="4" t="s">
         <v>39</v>
       </c>
@@ -1272,7 +1239,9 @@
         <v>25</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
         <v>40</v>
@@ -1493,13 +1462,13 @@
       <c r="N25" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B12 B15:B25 D2:N12 D15:N25">
-    <cfRule type="containsBlanks" dxfId="50" priority="2">
+  <conditionalFormatting sqref="B2:B12 B15:B25 D15:N25 D2:N12">
+    <cfRule type="containsBlanks" dxfId="28" priority="4">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C12 C15:C25">
-    <cfRule type="containsBlanks" dxfId="49" priority="1">
+    <cfRule type="containsBlanks" dxfId="27" priority="3">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1514,7 +1483,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q35" sqref="Q35"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1586,7 @@
         <v>51</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1941,138 +1910,138 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P6:T6 K2:T2 L8 K5:K6 K7:L7 B2:I8 N7:T8 K4:T4 K3:N3 P3:T3 P5:Q5 T5">
-    <cfRule type="containsBlanks" dxfId="48" priority="32">
+  <conditionalFormatting sqref="P6:T6 K2:T2 L8 K5:K6 K7:L7 N7:T8 K4:T4 K3:N3 P3:T3 P5:Q5 T5 B2:I8">
+    <cfRule type="containsBlanks" dxfId="26" priority="46">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:I12 B14:I15 K11:T12 K14:T15">
-    <cfRule type="containsBlanks" dxfId="47" priority="31">
+    <cfRule type="containsBlanks" dxfId="25" priority="45">
       <formula>LEN(TRIM(B11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16 E16:I16 L16:O16 R16:T16">
-    <cfRule type="containsBlanks" dxfId="46" priority="30">
+    <cfRule type="containsBlanks" dxfId="24" priority="44">
       <formula>LEN(TRIM(C16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:O5 L6 N6:O6">
-    <cfRule type="containsBlanks" dxfId="45" priority="29">
+    <cfRule type="containsBlanks" dxfId="23" priority="43">
       <formula>LEN(TRIM(L5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsBlanks" dxfId="44" priority="28">
+    <cfRule type="containsBlanks" dxfId="22" priority="42">
       <formula>LEN(TRIM(D16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsBlanks" dxfId="43" priority="27">
+    <cfRule type="containsBlanks" dxfId="21" priority="41">
       <formula>LEN(TRIM(B16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="containsBlanks" dxfId="42" priority="25">
+    <cfRule type="containsBlanks" dxfId="20" priority="39">
       <formula>LEN(TRIM(M6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16">
-    <cfRule type="containsBlanks" dxfId="41" priority="24">
+    <cfRule type="containsBlanks" dxfId="19" priority="38">
       <formula>LEN(TRIM(P16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J7">
-    <cfRule type="containsBlanks" dxfId="40" priority="23">
+    <cfRule type="containsBlanks" dxfId="18" priority="37">
       <formula>LEN(TRIM(J2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J12 J14:J15">
-    <cfRule type="containsBlanks" dxfId="39" priority="22">
+    <cfRule type="containsBlanks" dxfId="17" priority="36">
       <formula>LEN(TRIM(J11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="containsBlanks" dxfId="38" priority="20">
+    <cfRule type="containsBlanks" dxfId="16" priority="34">
       <formula>LEN(TRIM(J16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="containsBlanks" dxfId="37" priority="19">
+    <cfRule type="containsBlanks" dxfId="15" priority="33">
       <formula>LEN(TRIM(K16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:I17 L17 R17:T17 N17:P17">
-    <cfRule type="containsBlanks" dxfId="36" priority="18">
+    <cfRule type="containsBlanks" dxfId="14" priority="32">
       <formula>LEN(TRIM(C17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="containsBlanks" dxfId="34" priority="16">
+    <cfRule type="containsBlanks" dxfId="13" priority="30">
       <formula>LEN(TRIM(M7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:I13 K13:T13">
-    <cfRule type="containsBlanks" dxfId="33" priority="15">
+    <cfRule type="containsBlanks" dxfId="12" priority="29">
       <formula>LEN(TRIM(B13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="containsBlanks" dxfId="31" priority="14">
+    <cfRule type="containsBlanks" dxfId="11" priority="28">
       <formula>LEN(TRIM(J13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="containsBlanks" dxfId="29" priority="13">
+    <cfRule type="containsBlanks" dxfId="10" priority="27">
       <formula>LEN(TRIM(Q17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="containsBlanks" dxfId="23" priority="10">
+    <cfRule type="containsBlanks" dxfId="9" priority="24">
       <formula>LEN(TRIM(J17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="containsBlanks" dxfId="21" priority="9">
+    <cfRule type="containsBlanks" dxfId="8" priority="23">
       <formula>LEN(TRIM(K17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsBlanks" dxfId="19" priority="8">
+    <cfRule type="containsBlanks" dxfId="7" priority="22">
       <formula>LEN(TRIM(B17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="containsBlanks" dxfId="16" priority="7">
+    <cfRule type="containsBlanks" dxfId="6" priority="21">
       <formula>LEN(TRIM(K8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="containsBlanks" dxfId="14" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="20">
       <formula>LEN(TRIM(J8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsBlanks" dxfId="12" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="19">
       <formula>LEN(TRIM(M17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="containsBlanks" dxfId="10" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="18">
       <formula>LEN(TRIM(M8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
-    <cfRule type="containsBlanks" dxfId="7" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="17">
       <formula>LEN(TRIM(Q16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="containsBlanks" dxfId="5" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="16">
       <formula>LEN(TRIM(O3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:S5">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="15">
       <formula>LEN(TRIM(R5))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>